<commit_message>
update code bo phan phu cap tai cac co so khac
</commit_message>
<xml_diff>
--- a/Báo cáo/1_CẦN THƠ/Báo cáo cá nhân/NV-11 Đỗ Thị Huyền Trân 7-2024.xlsx
+++ b/Báo cáo/1_CẦN THƠ/Báo cáo cá nhân/NV-11 Đỗ Thị Huyền Trân 7-2024.xlsx
@@ -1988,7 +1988,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B40"/>
+  <dimension ref="A1:B38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2129,7 +2129,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Phụ cấp tại LONG XUYÊN</t>
+          <t>Lương công tác tại LONG XUYÊN</t>
         </is>
       </c>
       <c r="B14" t="n">
@@ -2139,27 +2139,27 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Lương công tác tại LONG XUYÊN</t>
+          <t>Lương cơ bản tại LONG XUYÊN</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>0</v>
+        <v/>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Lương cơ bản tại LONG XUYÊN</t>
+          <t>Chiết khấu sale chính tại LONG XUYÊN</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v/>
+        <v>0</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Chiết khấu sale chính tại LONG XUYÊN</t>
+          <t>Chiết khấu sale phụ tại LONG XUYÊN</t>
         </is>
       </c>
       <c r="B17" t="n">
@@ -2169,7 +2169,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Chiết khấu sale phụ tại LONG XUYÊN</t>
+          <t>Đơn 1 bác sĩ tại LONG XUYÊN</t>
         </is>
       </c>
       <c r="B18" t="n">
@@ -2179,7 +2179,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Đơn 1 bác sĩ tại LONG XUYÊN</t>
+          <t>Đơn 2 bác sĩ tại LONG XUYÊN</t>
         </is>
       </c>
       <c r="B19" t="n">
@@ -2189,7 +2189,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Đơn 2 bác sĩ tại LONG XUYÊN</t>
+          <t>Công phụ phẫu 1 tại LONG XUYÊN</t>
         </is>
       </c>
       <c r="B20" t="n">
@@ -2199,7 +2199,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Công phụ phẫu 1 tại LONG XUYÊN</t>
+          <t>Công phụ phẫu 2 tại LONG XUYÊN</t>
         </is>
       </c>
       <c r="B21" t="n">
@@ -2209,7 +2209,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Công phụ phẫu 2 tại LONG XUYÊN</t>
+          <t>Chiết khấu thu nợ tại LONG XUYÊN</t>
         </is>
       </c>
       <c r="B22" t="n">
@@ -2219,27 +2219,27 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Chiết khấu thu nợ tại LONG XUYÊN</t>
+          <t>Ứng lương tại LONG XUYÊN</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>0</v>
+        <v>-0</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Ứng lương tại LONG XUYÊN</t>
+          <t>Tổng công tại SÓC TRĂNG</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Tổng công tại SÓC TRĂNG</t>
+          <t>Lương công tác tại SÓC TRĂNG</t>
         </is>
       </c>
       <c r="B25" t="n">
@@ -2249,47 +2249,47 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Phụ cấp tại SÓC TRĂNG</t>
+          <t>Lương cơ bản tại SÓC TRĂNG</t>
         </is>
       </c>
       <c r="B26" t="n">
-        <v>0</v>
+        <v/>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Lương công tác tại SÓC TRĂNG</t>
+          <t>Chiết khấu sale chính tại SÓC TRĂNG</t>
         </is>
       </c>
       <c r="B27" t="n">
-        <v>0</v>
+        <v>120000</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Lương cơ bản tại SÓC TRĂNG</t>
+          <t>Chiết khấu sale phụ tại SÓC TRĂNG</t>
         </is>
       </c>
       <c r="B28" t="n">
-        <v/>
+        <v>0</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Chiết khấu sale chính tại SÓC TRĂNG</t>
+          <t>Đơn 1 bác sĩ tại SÓC TRĂNG</t>
         </is>
       </c>
       <c r="B29" t="n">
-        <v>120000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Chiết khấu sale phụ tại SÓC TRĂNG</t>
+          <t>Đơn 2 bác sĩ tại SÓC TRĂNG</t>
         </is>
       </c>
       <c r="B30" t="n">
@@ -2299,7 +2299,7 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Đơn 1 bác sĩ tại SÓC TRĂNG</t>
+          <t>Công phụ phẫu 1 tại SÓC TRĂNG</t>
         </is>
       </c>
       <c r="B31" t="n">
@@ -2309,7 +2309,7 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Đơn 2 bác sĩ tại SÓC TRĂNG</t>
+          <t>Công phụ phẫu 2 tại SÓC TRĂNG</t>
         </is>
       </c>
       <c r="B32" t="n">
@@ -2319,80 +2319,60 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Công phụ phẫu 1 tại SÓC TRĂNG</t>
+          <t>Chiết khấu thu nợ tại SÓC TRĂNG</t>
         </is>
       </c>
       <c r="B33" t="n">
-        <v>0</v>
+        <v>200000</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Công phụ phẫu 2 tại SÓC TRĂNG</t>
+          <t>Ứng lương tại SÓC TRĂNG</t>
         </is>
       </c>
       <c r="B34" t="n">
-        <v>0</v>
+        <v>-0</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Chiết khấu thu nợ tại SÓC TRĂNG</t>
+          <t>Tổng lương tại CẦN THƠ</t>
         </is>
       </c>
       <c r="B35" t="n">
-        <v>200000</v>
+        <v>10759000</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Ứng lương tại SÓC TRĂNG</t>
+          <t>Tổng lương tại LONG XUYÊN</t>
         </is>
       </c>
       <c r="B36" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Tổng lương tại CẦN THƠ</t>
+          <t>Tổng lương tại SÓC TRĂNG</t>
         </is>
       </c>
       <c r="B37" t="n">
-        <v>10759000</v>
+        <v>320000</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Tổng lương tại LONG XUYÊN</t>
+          <t>Tổng lương</t>
         </is>
       </c>
       <c r="B38" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39">
-      <c r="A39" t="inlineStr">
-        <is>
-          <t>Tổng lương tại SÓC TRĂNG</t>
-        </is>
-      </c>
-      <c r="B39" t="n">
-        <v>320000</v>
-      </c>
-    </row>
-    <row r="40">
-      <c r="A40" t="inlineStr">
-        <is>
-          <t>Tổng lương</t>
-        </is>
-      </c>
-      <c r="B40" t="n">
         <v>11079000</v>
       </c>
     </row>

</xml_diff>